<commit_message>
Update 16 May: add new uploads
</commit_message>
<xml_diff>
--- a/uploads/track/qxzyolhv3.xlsx
+++ b/uploads/track/qxzyolhv3.xlsx
@@ -11,12 +11,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>આપનું નામ</t>
   </si>
   <si>
     <t>hkjhkhkjh</t>
+  </si>
+  <si>
+    <t>sdfsf</t>
   </si>
 </sst>
 </file>
@@ -393,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -406,8 +409,13 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>